<commit_message>
results - duration part finalized
</commit_message>
<xml_diff>
--- a/Tables/Table_S3.xlsx
+++ b/Tables/Table_S3.xlsx
@@ -415,14 +415,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>9.32</t>
+          <t>9.74</t>
         </is>
       </c>
       <c r="F2">
-        <v>-9.699999999999999</v>
+        <v>-9.26</v>
       </c>
       <c r="G2">
-        <v>29.15</v>
+        <v>28.03</v>
       </c>
     </row>
     <row r="3">
@@ -446,14 +446,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5.52</t>
+          <t>4.77</t>
         </is>
       </c>
       <c r="F3">
-        <v>-17.91</v>
+        <v>-18.65</v>
       </c>
       <c r="G3">
-        <v>28.52</v>
+        <v>28.32</v>
       </c>
     </row>
     <row r="4">
@@ -477,14 +477,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3.23</t>
+          <t>3.79</t>
         </is>
       </c>
       <c r="F4">
-        <v>-25.5</v>
+        <v>-26.73</v>
       </c>
       <c r="G4">
-        <v>33.46</v>
+        <v>33.21</v>
       </c>
     </row>
     <row r="5">
@@ -508,14 +508,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-6.82</t>
+          <t>-6.5</t>
         </is>
       </c>
       <c r="F5">
-        <v>-31.01</v>
+        <v>-30.32</v>
       </c>
       <c r="G5">
-        <v>18.2</v>
+        <v>17.57</v>
       </c>
     </row>
     <row r="6">
@@ -644,10 +644,10 @@
         </is>
       </c>
       <c r="F10">
-        <v>-0.35</v>
+        <v>-0.37</v>
       </c>
       <c r="G10">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="11">
@@ -675,10 +675,10 @@
         </is>
       </c>
       <c r="F11">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="G11">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="12">
@@ -733,11 +733,11 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-0.14</t>
+          <t>-0.13</t>
         </is>
       </c>
       <c r="F13">
-        <v>-0.26</v>
+        <v>-0.25</v>
       </c>
       <c r="G13">
         <v>-0.01</v>
@@ -764,11 +764,11 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="F14">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="G14">
         <v>0.2</v>
@@ -865,11 +865,11 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2.58</t>
+          <t>2.59</t>
         </is>
       </c>
       <c r="F18">
-        <v>2.11</v>
+        <v>2.1</v>
       </c>
       <c r="G18">
         <v>3.05</v>
@@ -896,7 +896,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.48</t>
         </is>
       </c>
       <c r="F19">
@@ -927,11 +927,11 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-0.02</t>
+          <t>-0.01</t>
         </is>
       </c>
       <c r="F20">
-        <v>-0.5</v>
+        <v>-0.49</v>
       </c>
       <c r="G20">
         <v>0.47</v>
@@ -958,11 +958,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-0.18</t>
+          <t>-0.19</t>
         </is>
       </c>
       <c r="F21">
-        <v>-0.75</v>
+        <v>-0.77</v>
       </c>
       <c r="G21">
         <v>0.39</v>
@@ -1059,14 +1059,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>12.06</t>
+          <t>11.98</t>
         </is>
       </c>
       <c r="F25">
-        <v>7.67</v>
+        <v>7.78</v>
       </c>
       <c r="G25">
-        <v>16.24</v>
+        <v>16.12</v>
       </c>
     </row>
     <row r="26">
@@ -1090,14 +1090,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-0.6</t>
+          <t>-0.56</t>
         </is>
       </c>
       <c r="F26">
-        <v>-5.99</v>
+        <v>-5.92</v>
       </c>
       <c r="G26">
-        <v>4.94</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="27">
@@ -1121,14 +1121,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>13.85</t>
+          <t>13.82</t>
         </is>
       </c>
       <c r="F27">
-        <v>2.82</v>
+        <v>2.34</v>
       </c>
       <c r="G27">
-        <v>25.37</v>
+        <v>25.45</v>
       </c>
     </row>
     <row r="28">
@@ -1152,14 +1152,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-4.52</t>
+          <t>-4.47</t>
         </is>
       </c>
       <c r="F28">
-        <v>-9</v>
+        <v>-8.970000000000001</v>
       </c>
       <c r="G28">
-        <v>-0.02</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="29">
@@ -1183,14 +1183,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>9.17</t>
+          <t>9.49</t>
         </is>
       </c>
       <c r="F29">
-        <v>-9.289999999999999</v>
+        <v>-8.93</v>
       </c>
       <c r="G29">
-        <v>27.6</v>
+        <v>27.64</v>
       </c>
     </row>
     <row r="30">
@@ -1214,14 +1214,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1.95</t>
         </is>
       </c>
       <c r="F30">
-        <v>-3.32</v>
+        <v>-3.44</v>
       </c>
       <c r="G30">
-        <v>7.38</v>
+        <v>7.43</v>
       </c>
     </row>
     <row r="31">

</xml_diff>